<commit_message>
Fixed component orientations is CPL file.
</commit_message>
<xml_diff>
--- a/v0p3/gerber_v0p3_r1/BOM_JLCPCB.xlsx
+++ b/v0p3/gerber_v0p3_r1/BOM_JLCPCB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -125,19 +125,13 @@
     <t xml:space="preserve">C190321</t>
   </si>
   <si>
-    <t xml:space="preserve">ADG702 SPST-NC switch</t>
+    <t xml:space="preserve">TS5A3160 SPDT Analog Switch</t>
   </si>
   <si>
     <t xml:space="preserve">U2</t>
   </si>
   <si>
     <t xml:space="preserve">SOT-23-6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C133478</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS5A3160 SPDT Analog Switch</t>
   </si>
   <si>
     <t xml:space="preserve">C185770</t>
@@ -383,7 +377,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -513,42 +507,26 @@
       <c r="E7" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -561,7 +539,7 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>